<commit_message>
New version of function access
Small changes and new lines of code in all functions:
-Added case 3 of subsamples.
-Added fill gaps in non target species L W
-Changes in visualization of several plot in perform checks
-Changes in PDF generation
-Added target species CALLSAP in excel file
</commit_message>
<xml_diff>
--- a/OnBoard/data/target_species.xlsx
+++ b/OnBoard/data/target_species.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1bcb1d8ec36d6377/Lavoro/Solemon/github/SoleMon_project/OnBoard/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.palermino\OneDrive - CNR\github\SoleMon_project\OnBoard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{1E0423C8-0D40-4309-BF0E-4154ECF0BACF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228"/>
   </bookViews>
   <sheets>
     <sheet name="target_species" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>species_name</t>
   </si>
@@ -116,12 +115,15 @@
   </si>
   <si>
     <t>GALEECH</t>
+  </si>
+  <si>
+    <t>CALLSAP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -603,48 +605,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Calcolo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cella collegata" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Cella da controllare" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Colore 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Colore 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Colore 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Colore 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Colore 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Colore 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Neutrale" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Testo avviso" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Testo descrittivo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titolo" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titolo 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titolo 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titolo 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titolo 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Totale" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Valore non valido" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Valore valido" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -955,20 +957,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -976,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -984,7 +986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -992,7 +994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1000,7 +1002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1008,7 +1010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1016,7 +1018,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1024,7 +1026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1032,7 +1034,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1040,7 +1042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1048,7 +1050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1056,7 +1058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1064,7 +1066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1072,7 +1074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1080,7 +1082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1088,7 +1090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1096,7 +1098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1104,7 +1106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1112,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1120,7 +1122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1128,7 +1130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1136,7 +1138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1144,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1152,7 +1154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -1160,7 +1162,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -1168,7 +1170,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1176,7 +1178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -1184,7 +1186,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1192,7 +1194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -1200,7 +1202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1208,12 +1210,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31">
         <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>